<commit_message>
update learning curve for report
</commit_message>
<xml_diff>
--- a/outputs/final report/Hyperparameter_Tuning_Results_FINAL.xlsx
+++ b/outputs/final report/Hyperparameter_Tuning_Results_FINAL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepo\Go3D\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepo\Go3D\outputs\final report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392A771E-7884-4692-AFE9-502D9CE1FC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C694BDB3-5395-4511-A81E-3D8AABB2D631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-3600" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <customWorkbookView name="Filter 1" guid="{090C84B6-707E-4C3B-9D95-45B567422621}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -491,10 +491,10 @@
     <t>PointNet</t>
   </si>
   <si>
-    <t>Ours</t>
-  </si>
-  <si>
     <t>Overfitting Index</t>
+  </si>
+  <si>
+    <t>Go3D</t>
   </si>
 </sst>
 </file>
@@ -697,45 +697,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000%"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2160,7 +2136,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{586F88F2-9477-4658-BD66-3E973DE604BD}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="7" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{586F88F2-9477-4658-BD66-3E973DE604BD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="7" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -2223,7 +2199,7 @@
     <dataField name="Max of VALIDATE ACCURACY" fld="11" subtotal="max" baseField="6" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2440,7 +2416,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2474,21 +2450,21 @@
       <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27" t="s">
+      <c r="J3" s="28"/>
+      <c r="K3" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -2500,29 +2476,29 @@
       <c r="C4" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="28" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="N4" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="26" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2536,31 +2512,31 @@
       <c r="C5" s="17">
         <v>0.86233478784561102</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="26">
         <v>0.86319220066070501</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="26">
         <v>0.86563879251480103</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="26">
         <v>1024</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="26">
         <v>32</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="26">
         <v>24</v>
       </c>
-      <c r="N5" s="28" t="b">
+      <c r="N5" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="26">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="26">
         <v>0.3</v>
       </c>
     </row>
@@ -2574,31 +2550,31 @@
       <c r="C6" s="17">
         <v>0.86563879251480103</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="I6" s="28">
+      <c r="H6" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6" s="26">
         <v>0.86018544435501099</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="26">
         <v>0.86233478784561102</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="26">
         <v>1024</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="26">
         <v>32</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="26">
         <v>24</v>
       </c>
-      <c r="N6" s="28" t="b">
+      <c r="N6" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="O6" s="28">
+      <c r="O6" s="26">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="26">
         <v>0.3</v>
       </c>
     </row>
@@ -2675,7 +2651,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -2972,7 +2948,7 @@
         <v>-2.3561470927992108E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -3014,7 +2990,7 @@
         <v>0.15200350527746928</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3056,7 +3032,7 @@
         <v>6.2631264398589105E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -3098,7 +3074,7 @@
         <v>-4.0195238847352812E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -3140,7 +3116,7 @@
         <v>6.5065759614531066E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -3476,7 +3452,7 @@
         <v>5.6726129075369565E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -3518,7 +3494,7 @@
         <v>0.11864177327854354</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -3560,7 +3536,7 @@
         <v>-5.07076934845939E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -3602,7 +3578,7 @@
         <v>3.9722670815608464E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
@@ -3644,7 +3620,7 @@
         <v>0.19606307184419669</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
@@ -3980,7 +3956,7 @@
         <v>3.2211133422565159E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -4022,7 +3998,7 @@
         <v>3.2877098958211878E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
@@ -4064,7 +4040,7 @@
         <v>5.6595992508970634E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -4106,7 +4082,7 @@
         <v>1.240444219631128E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
@@ -4148,7 +4124,7 @@
         <v>0.11253014634023913</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>48</v>
       </c>
@@ -6272,7 +6248,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" s="8">
         <v>1024</v>
       </c>
@@ -6302,7 +6278,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" s="8">
         <v>1024</v>
       </c>
@@ -6332,7 +6308,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" s="8">
         <v>1024</v>
       </c>
@@ -6362,7 +6338,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" s="8">
         <v>1024</v>
       </c>
@@ -6392,7 +6368,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="97" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:13" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" s="8">
         <v>1024</v>
       </c>
@@ -6422,7 +6398,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="570" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="570" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J570" s="2" t="s">
         <v>86</v>
       </c>
@@ -6438,7 +6414,7 @@
   <customSheetViews>
     <customSheetView guid="{090C84B6-707E-4C3B-9D95-45B567422621}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:Y97" xr:uid="{5EBDCBAE-4725-44C2-9F69-050CCE16C4D6}">
+      <autoFilter ref="A1:Y97" xr:uid="{03E7EE4C-7A3C-4110-93AD-27E69820C643}">
         <filterColumn colId="3">
           <filters>
             <filter val="32"/>
@@ -6568,7 +6544,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>116</v>
       </c>

</xml_diff>